<commit_message>
New Test Case added SPcartCheck Add items
</commit_message>
<xml_diff>
--- a/hybris-nao-tests/src/main/resources/SingleInputTestData.xlsx
+++ b/hybris-nao-tests/src/main/resources/SingleInputTestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\seleniumAutomationScripts\hybris\hyb4nov18\hybNov62017\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rajkumars\git\IRWWebservice\hybris-nao-tests\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0CE979B-EBBA-44FE-8896-523D68CABD61}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D607B4B-14C8-4E88-B6EF-2E902BB8DB19}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="5730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15" yWindow="15" windowWidth="20460" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Case" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="225">
   <si>
     <t>TCID</t>
   </si>
@@ -703,6 +703,12 @@
   </si>
   <si>
     <t>Validate quick order values to Shopping cart values</t>
+  </si>
+  <si>
+    <t>SPCartItemsAddCheckTest</t>
+  </si>
+  <si>
+    <t>Validate Shopping cart Add item verification  test</t>
   </si>
 </sst>
 </file>
@@ -762,7 +768,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -798,23 +804,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -829,7 +824,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1182,10 +1176,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1830,13 +1824,13 @@
       <c r="A46" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="B46" s="12" t="s">
+      <c r="B46" s="9" t="s">
         <v>216</v>
       </c>
-      <c r="C46" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="D46" s="12" t="s">
+      <c r="C46" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="D46" s="9" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1844,13 +1838,13 @@
       <c r="A47" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="B47" s="12" t="s">
+      <c r="B47" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="C47" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="D47" s="12" t="s">
+      <c r="C47" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="D47" s="9" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1858,13 +1852,13 @@
       <c r="A48" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="B48" s="12" t="s">
+      <c r="B48" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="C48" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="D48" s="12" t="s">
+      <c r="C48" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="D48" s="9" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1872,13 +1866,27 @@
       <c r="A49" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="B49" s="12" t="s">
+      <c r="B49" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="C49" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="D49" s="12" t="s">
+      <c r="C49" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="D49" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="D50" s="9" t="s">
         <v>101</v>
       </c>
     </row>

</xml_diff>